<commit_message>
add 11th table and trend lines in tableau
</commit_message>
<xml_diff>
--- a/01 Data/city_temp_info.xlsx
+++ b/01 Data/city_temp_info.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="135">
   <si>
     <t>Number</t>
   </si>
@@ -419,6 +420,12 @@
   </si>
   <si>
     <t>Avg_temp_max</t>
+  </si>
+  <si>
+    <t>Avg_temp_min_2014</t>
+  </si>
+  <si>
+    <t>Avg_temp_max_2014</t>
   </si>
 </sst>
 </file>
@@ -467,8 +474,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -477,11 +524,51 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -813,8 +900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:A8"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108:XFD108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3784,6 +3871,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3796,8 +3884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6082,4 +6170,261 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>23090</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>34.92</v>
+      </c>
+      <c r="D2">
+        <v>138.62</v>
+      </c>
+      <c r="E2">
+        <v>48</v>
+      </c>
+      <c r="F2">
+        <v>12.84</v>
+      </c>
+      <c r="G2">
+        <v>23.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>40842</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>27.39</v>
+      </c>
+      <c r="D3">
+        <v>153.13</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>16.170000000000002</v>
+      </c>
+      <c r="G3">
+        <v>25.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>31011</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>16.87</v>
+      </c>
+      <c r="D4">
+        <v>145.75</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>20.8</v>
+      </c>
+      <c r="G4">
+        <v>29.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>70351</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>35.31</v>
+      </c>
+      <c r="D5">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="E5">
+        <v>577</v>
+      </c>
+      <c r="F5">
+        <v>6.69</v>
+      </c>
+      <c r="G5">
+        <v>21.47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>14015</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>12.42</v>
+      </c>
+      <c r="D6">
+        <v>130.88999999999999</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>22.98</v>
+      </c>
+      <c r="G6">
+        <v>32.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>94029</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7">
+        <v>42.89</v>
+      </c>
+      <c r="D7">
+        <v>147.33000000000001</v>
+      </c>
+      <c r="E7">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="G7">
+        <v>18.260000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>86071</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8">
+        <v>37.81</v>
+      </c>
+      <c r="D8">
+        <v>144.97</v>
+      </c>
+      <c r="E8">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <v>12.42</v>
+      </c>
+      <c r="G8">
+        <v>21.66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>66062</v>
+      </c>
+      <c r="B9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9">
+        <v>33.86</v>
+      </c>
+      <c r="D9">
+        <v>151.21</v>
+      </c>
+      <c r="E9">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>15.11</v>
+      </c>
+      <c r="G9">
+        <v>23.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>32040</v>
+      </c>
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10">
+        <v>19.25</v>
+      </c>
+      <c r="D10">
+        <v>146.77000000000001</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>20.23</v>
+      </c>
+      <c r="G10">
+        <v>29.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>